<commit_message>
update timesheet + add 5th sitrep
</commit_message>
<xml_diff>
--- a/time-sheet.xlsx
+++ b/time-sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14220" tabRatio="500"/>
+    <workbookView xWindow="5260" yWindow="540" windowWidth="25600" windowHeight="14220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,16 +18,28 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -50,14 +62,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -387,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -483,8 +499,17 @@
         <v>11</v>
       </c>
     </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1">
+        <v>41641</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>